<commit_message>
All other regions added, 20 minute surrenders, <20 minute games, more info in About page.
</commit_message>
<xml_diff>
--- a/site/brawlers.xlsx
+++ b/site/brawlers.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
@@ -88,7 +88,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -387,7 +387,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,34 +432,34 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>31.51</v>
+        <v>29.91</v>
       </c>
       <c r="B2">
-        <v>16.04</v>
+        <v>15.64</v>
       </c>
       <c r="C2">
-        <v>11.26</v>
+        <v>11.56</v>
       </c>
       <c r="D2">
-        <v>5.5</v>
+        <v>5.86</v>
       </c>
       <c r="E2">
-        <v>2.72</v>
+        <v>4.25</v>
       </c>
       <c r="F2">
-        <v>50.99</v>
+        <v>51.01</v>
       </c>
       <c r="G2">
-        <v>49.96</v>
+        <v>50.35</v>
       </c>
       <c r="H2">
-        <v>50.61</v>
+        <v>50.97</v>
       </c>
       <c r="I2">
-        <v>48.19</v>
+        <v>48.43</v>
       </c>
       <c r="J2">
-        <v>41.57</v>
+        <v>39.67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>